<commit_message>
addressed points of PR #15, changed emdataset base, added back Readme to examples
</commit_message>
<xml_diff>
--- a/project/spa/excel/oscem_schemas_spa.xlsx
+++ b/project/spa/excel/oscem_schemas_spa.xlsx
@@ -942,7 +942,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>molecular_type</t>
+          <t>molecular_overall_type</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -967,7 +967,10 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="2">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"CELL,COMPLEX,ORGANELLE OR CELLULAR COMPONENT,RIBOSOME,TISSUE,VIRUS"</formula1>
+    </dataValidation>
     <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"FILAMENT,HELICAL ARRAY,PARTICLE"</formula1>
     </dataValidation>
@@ -1038,11 +1041,6 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"CELL,COMPLEX,ORGANELLE OR CELLULAR COMPONENT,RIBOSOME,TISSUE,VIRUS"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
circumvented reliance on any_of for quantitySI
</commit_message>
<xml_diff>
--- a/project/spa/excel/oscem_schemas_spa.xlsx
+++ b/project/spa/excel/oscem_schemas_spa.xlsx
@@ -1645,6 +1645,47 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>particles_per_2Dclass</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>images_classes_2D</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>resolution_classes_2D</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>descriptors</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1656,22 +1697,22 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>number_classes_2D</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>particles_per_2Dclass</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>images_classes_2D</t>
+          <t>particles_per_3Dclass</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>images_classes_3D</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>volume</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>resolution_classes_2D</t>
+          <t>resolution_classes_3D</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
@@ -1685,48 +1726,156 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>number_classes_3D</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>particles_per_3Dclass</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>images_classes_3D</t>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>orthogonal_slices</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>isosurface_images</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>orthogonal_slices_X</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>orthogonal_slices_Y</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>orthogonal_slices_Z</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>front_view</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>side_view</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>top_view</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>volume_type</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>vol_number_particles</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>size</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>volume</t>
+          <t>orthogonal_slices</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>resolution_classes_3D</t>
+          <t>isosurface_images</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>vol_resolution</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
           <t>descriptors</t>
         </is>
       </c>
@@ -1736,7 +1885,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1753,93 +1902,21 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>orthogonal_slices</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>isosurface_images</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>orthogonal_slices_X</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>orthogonal_slices_Y</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>orthogonal_slices_Z</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>front_view</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>side_view</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>top_view</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+          <t>height</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>width</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1856,46 +1933,133 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>volume_type</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>vol_number_particles</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>size</t>
+          <t>movies</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>micrographs</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>ctfs</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>orthogonal_slices</t>
+          <t>coordinates</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>isosurface_images</t>
+          <t>classes2D</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>vol_resolution</t>
+          <t>classes3D</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>descriptors</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+          <t>volumes</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>processing</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>acquisition</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>instrument</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>organizational</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>x_min</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>x_max</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>y_min</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>y_max</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1912,313 +2076,139 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>height</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>width</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>movies</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>micrographs</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>ctfs</t>
+          <t>unit</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>valueSI</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>unitSI</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>unit</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>coordinates</t>
+          <t>value</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>descriptor_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>descriptor_thing</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AA1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>nominal_defocus</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>calibrated_defocus</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>nominal_magnification</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>calibrated_magnification</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>classes2D</t>
+          <t>holder</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>classes3D</t>
+          <t>holder_cryogen</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>volumes</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>processing</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>acquisition</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>instrument</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>organizational</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>x_min</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>x_max</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>y_min</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>y_max</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>unit</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>value</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>valueSI</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>unitSI</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>unit</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>value</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>descriptor_name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>descriptor_thing</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AA1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>nominal_defocus</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>calibrated_defocus</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>nominal_magnification</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>calibrated_magnification</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>holder</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>holder_cryogen</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
           <t>temperature_range</t>
         </is>
       </c>

</xml_diff>